<commit_message>
start of OSPC presentation
</commit_message>
<xml_diff>
--- a/Data/Calibration/CalibrationTables.xlsx
+++ b/Data/Calibration/CalibrationTables.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="24816"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="25516"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="-20" yWindow="0" windowWidth="25040" windowHeight="14920" tabRatio="500" firstSheet="4" activeTab="4"/>
+    <workbookView xWindow="560" yWindow="560" windowWidth="25040" windowHeight="14980" tabRatio="500" firstSheet="4" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="SupplySideVariableList" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="332" uniqueCount="216">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="331" uniqueCount="215">
   <si>
     <t>Parameter</t>
   </si>
@@ -334,15 +334,9 @@
     <t>Public Administration</t>
   </si>
   <si>
-    <t>Inudstry Number</t>
-  </si>
-  <si>
     <t>Industry</t>
   </si>
   <si>
-    <t>Good Number</t>
-  </si>
-  <si>
     <t>Consumption Good Category</t>
   </si>
   <si>
@@ -674,6 +668,9 @@
   </si>
   <si>
     <t>NAICS Code</t>
+  </si>
+  <si>
+    <t>Industry Number</t>
   </si>
 </sst>
 </file>
@@ -734,7 +731,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="12">
+  <cellStyleXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -747,6 +744,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
@@ -754,12 +752,13 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="12">
+  <cellStyles count="13">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="8" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="10" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="12" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -1295,7 +1294,7 @@
     </row>
     <row r="27" spans="1:2">
       <c r="A27" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="B27" t="s">
         <v>38</v>
@@ -1303,7 +1302,7 @@
     </row>
     <row r="28" spans="1:2">
       <c r="A28" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
       <c r="B28" t="s">
         <v>77</v>
@@ -1311,15 +1310,15 @@
     </row>
     <row r="29" spans="1:2">
       <c r="A29" t="s">
-        <v>207</v>
+        <v>205</v>
       </c>
     </row>
     <row r="30" spans="1:2">
       <c r="A30" t="s">
-        <v>208</v>
+        <v>206</v>
       </c>
       <c r="B30" t="s">
-        <v>209</v>
+        <v>207</v>
       </c>
     </row>
   </sheetData>
@@ -1358,7 +1357,7 @@
     </row>
     <row r="4" spans="1:2">
       <c r="A4" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
       <c r="B4" t="s">
         <v>54</v>
@@ -1366,7 +1365,7 @@
     </row>
     <row r="5" spans="1:2">
       <c r="A5" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
       <c r="B5" t="s">
         <v>55</v>
@@ -1374,7 +1373,7 @@
     </row>
     <row r="6" spans="1:2">
       <c r="A6" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
       <c r="B6" t="s">
         <v>56</v>
@@ -1382,7 +1381,7 @@
     </row>
     <row r="7" spans="1:2">
       <c r="A7" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
       <c r="B7" t="s">
         <v>57</v>
@@ -1390,7 +1389,7 @@
     </row>
     <row r="8" spans="1:2">
       <c r="A8" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
       <c r="B8" t="s">
         <v>58</v>
@@ -1403,7 +1402,7 @@
     </row>
     <row r="10" spans="1:2">
       <c r="A10" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
       <c r="B10" t="s">
         <v>61</v>
@@ -1411,7 +1410,7 @@
     </row>
     <row r="11" spans="1:2">
       <c r="A11" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
       <c r="B11" t="s">
         <v>62</v>
@@ -1419,7 +1418,7 @@
     </row>
     <row r="12" spans="1:2">
       <c r="A12" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
       <c r="B12" t="s">
         <v>63</v>
@@ -1427,7 +1426,7 @@
     </row>
     <row r="13" spans="1:2">
       <c r="A13" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
       <c r="B13" t="s">
         <v>64</v>
@@ -1435,7 +1434,7 @@
     </row>
     <row r="14" spans="1:2">
       <c r="A14" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
       <c r="B14" t="s">
         <v>65</v>
@@ -1443,7 +1442,7 @@
     </row>
     <row r="15" spans="1:2">
       <c r="A15" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
       <c r="B15" t="s">
         <v>66</v>
@@ -1451,7 +1450,7 @@
     </row>
     <row r="16" spans="1:2">
       <c r="A16" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
       <c r="B16" t="s">
         <v>70</v>
@@ -1464,7 +1463,7 @@
     </row>
     <row r="18" spans="1:2">
       <c r="A18" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
       <c r="B18" t="s">
         <v>68</v>
@@ -1472,7 +1471,7 @@
     </row>
     <row r="19" spans="1:2">
       <c r="A19" t="s">
-        <v>194</v>
+        <v>192</v>
       </c>
       <c r="B19" t="s">
         <v>69</v>
@@ -1480,7 +1479,7 @@
     </row>
     <row r="20" spans="1:2">
       <c r="A20" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="B20" t="s">
         <v>72</v>
@@ -1493,7 +1492,7 @@
     </row>
     <row r="22" spans="1:2">
       <c r="A22" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
       <c r="B22" t="s">
         <v>75</v>
@@ -1501,7 +1500,7 @@
     </row>
     <row r="23" spans="1:2">
       <c r="A23" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
       <c r="B23" t="s">
         <v>74</v>
@@ -1509,7 +1508,7 @@
     </row>
     <row r="24" spans="1:2">
       <c r="A24" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
       <c r="B24" t="s">
         <v>76</v>
@@ -1517,7 +1516,7 @@
     </row>
     <row r="25" spans="1:2">
       <c r="A25" t="s">
-        <v>199</v>
+        <v>197</v>
       </c>
       <c r="B25" t="s">
         <v>78</v>
@@ -1525,7 +1524,7 @@
     </row>
     <row r="26" spans="1:2">
       <c r="A26" t="s">
-        <v>200</v>
+        <v>198</v>
       </c>
       <c r="B26" t="s">
         <v>79</v>
@@ -1533,7 +1532,7 @@
     </row>
     <row r="27" spans="1:2">
       <c r="A27" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
       <c r="B27" t="s">
         <v>80</v>
@@ -1568,51 +1567,51 @@
         <v>1</v>
       </c>
       <c r="C2" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
     </row>
     <row r="3" spans="1:3">
       <c r="A3" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
       <c r="B3" t="s">
         <v>33</v>
       </c>
       <c r="C3" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
     </row>
     <row r="4" spans="1:3">
       <c r="A4" t="s">
-        <v>203</v>
+        <v>201</v>
       </c>
       <c r="B4" t="s">
         <v>34</v>
       </c>
       <c r="C4" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
     </row>
     <row r="5" spans="1:3">
       <c r="A5" t="s">
-        <v>204</v>
+        <v>202</v>
       </c>
       <c r="B5" t="s">
         <v>35</v>
       </c>
       <c r="C5" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
     </row>
     <row r="6" spans="1:3">
       <c r="A6" t="s">
+        <v>208</v>
+      </c>
+      <c r="B6" t="s">
+        <v>209</v>
+      </c>
+      <c r="C6" t="s">
         <v>210</v>
-      </c>
-      <c r="B6" t="s">
-        <v>211</v>
-      </c>
-      <c r="C6" t="s">
-        <v>212</v>
       </c>
     </row>
   </sheetData>
@@ -1649,7 +1648,7 @@
     </row>
     <row r="3" spans="1:3">
       <c r="A3" t="s">
-        <v>205</v>
+        <v>203</v>
       </c>
       <c r="B3" t="s">
         <v>51</v>
@@ -1660,7 +1659,7 @@
     </row>
     <row r="4" spans="1:3">
       <c r="A4" t="s">
-        <v>206</v>
+        <v>204</v>
       </c>
       <c r="B4" t="s">
         <v>53</v>
@@ -1684,20 +1683,20 @@
   <dimension ref="A1:C25"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C25" sqref="A1:C25"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <sheetData>
     <row r="1" spans="1:3">
       <c r="A1" t="s">
+        <v>214</v>
+      </c>
+      <c r="B1" t="s">
+        <v>213</v>
+      </c>
+      <c r="C1" t="s">
         <v>102</v>
-      </c>
-      <c r="B1" t="s">
-        <v>215</v>
-      </c>
-      <c r="C1" t="s">
-        <v>103</v>
       </c>
     </row>
     <row r="2" spans="1:3" ht="16">
@@ -1719,7 +1718,7 @@
         <v>211</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
     </row>
     <row r="4" spans="1:3" ht="16">
@@ -1727,10 +1726,10 @@
         <v>3</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
     </row>
     <row r="5" spans="1:3" ht="16">
@@ -1763,7 +1762,7 @@
         <v>32411</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
     </row>
     <row r="8" spans="1:3" ht="16">
@@ -1774,7 +1773,7 @@
         <v>336</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
     </row>
     <row r="9" spans="1:3" ht="16">
@@ -1785,7 +1784,7 @@
         <v>3391</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
     </row>
     <row r="10" spans="1:3" ht="16">
@@ -1793,7 +1792,7 @@
         <v>9</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="C10" s="2" t="s">
         <v>84</v>
@@ -2008,11 +2007,8 @@
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <sheetData>
     <row r="1" spans="1:2">
-      <c r="A1" t="s">
-        <v>104</v>
-      </c>
       <c r="B1" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
     </row>
     <row r="2" spans="1:2">
@@ -2020,7 +2016,7 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
     </row>
     <row r="3" spans="1:2">
@@ -2028,7 +2024,7 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
     </row>
     <row r="4" spans="1:2">
@@ -2036,7 +2032,7 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
     </row>
     <row r="5" spans="1:2">
@@ -2044,7 +2040,7 @@
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
     </row>
     <row r="6" spans="1:2">
@@ -2052,7 +2048,7 @@
         <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
     </row>
     <row r="7" spans="1:2">
@@ -2060,7 +2056,7 @@
         <v>6</v>
       </c>
       <c r="B7" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
     </row>
     <row r="8" spans="1:2">
@@ -2068,7 +2064,7 @@
         <v>7</v>
       </c>
       <c r="B8" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
     </row>
     <row r="9" spans="1:2">
@@ -2076,7 +2072,7 @@
         <v>8</v>
       </c>
       <c r="B9" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
     </row>
     <row r="10" spans="1:2">
@@ -2084,7 +2080,7 @@
         <v>9</v>
       </c>
       <c r="B10" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
     </row>
     <row r="11" spans="1:2">
@@ -2092,7 +2088,7 @@
         <v>10</v>
       </c>
       <c r="B11" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
     </row>
     <row r="12" spans="1:2">
@@ -2100,7 +2096,7 @@
         <v>11</v>
       </c>
       <c r="B12" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
     </row>
     <row r="13" spans="1:2">
@@ -2108,7 +2104,7 @@
         <v>12</v>
       </c>
       <c r="B13" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
     </row>
     <row r="14" spans="1:2">
@@ -2116,7 +2112,7 @@
         <v>13</v>
       </c>
       <c r="B14" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
     </row>
     <row r="15" spans="1:2">
@@ -2124,7 +2120,7 @@
         <v>14</v>
       </c>
       <c r="B15" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
     </row>
     <row r="16" spans="1:2">
@@ -2132,7 +2128,7 @@
         <v>15</v>
       </c>
       <c r="B16" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
     </row>
     <row r="17" spans="1:2">
@@ -2140,7 +2136,7 @@
         <v>16</v>
       </c>
       <c r="B17" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
     </row>
     <row r="18" spans="1:2">
@@ -2148,7 +2144,7 @@
         <v>17</v>
       </c>
       <c r="B18" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
     </row>
   </sheetData>
@@ -2181,13 +2177,13 @@
         <v>0</v>
       </c>
       <c r="B2" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="C2" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="D2" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="E2" t="s">
         <v>1</v>
@@ -2203,10 +2199,10 @@
         <v>40</v>
       </c>
       <c r="B4" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="C4" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="E4" t="s">
         <v>3</v>
@@ -2217,7 +2213,7 @@
         <v>41</v>
       </c>
       <c r="B5" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="E5" t="s">
         <v>4</v>
@@ -2228,10 +2224,10 @@
         <v>42</v>
       </c>
       <c r="B6" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="C6" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="E6" t="s">
         <v>5</v>
@@ -2242,7 +2238,7 @@
         <v>43</v>
       </c>
       <c r="B7" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="E7" t="s">
         <v>6</v>
@@ -2253,7 +2249,7 @@
         <v>44</v>
       </c>
       <c r="B8" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="E8" t="s">
         <v>7</v>
@@ -2269,7 +2265,7 @@
         <v>9</v>
       </c>
       <c r="B10" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="E10" t="s">
         <v>45</v>
@@ -2280,7 +2276,7 @@
         <v>71</v>
       </c>
       <c r="B11" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="E11" t="s">
         <v>46</v>
@@ -2296,10 +2292,10 @@
         <v>47</v>
       </c>
       <c r="B13" t="s">
+        <v>137</v>
+      </c>
+      <c r="D13" t="s">
         <v>139</v>
-      </c>
-      <c r="D13" t="s">
-        <v>141</v>
       </c>
       <c r="E13" t="s">
         <v>11</v>
@@ -2310,10 +2306,10 @@
         <v>48</v>
       </c>
       <c r="B14" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="C14" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="E14" t="s">
         <v>12</v>
@@ -2329,7 +2325,7 @@
         <v>14</v>
       </c>
       <c r="B16" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="E16" t="s">
         <v>15</v>
@@ -2340,10 +2336,10 @@
         <v>49</v>
       </c>
       <c r="B17" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="C17" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="E17" t="s">
         <v>16</v>
@@ -2354,7 +2350,7 @@
         <v>17</v>
       </c>
       <c r="B18" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="E18" t="s">
         <v>18</v>
@@ -2365,7 +2361,7 @@
         <v>19</v>
       </c>
       <c r="B19" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="E19" t="s">
         <v>20</v>
@@ -2376,7 +2372,7 @@
         <v>21</v>
       </c>
       <c r="B20" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="E20" t="s">
         <v>22</v>
@@ -2387,7 +2383,7 @@
         <v>23</v>
       </c>
       <c r="B21" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="E21" t="s">
         <v>24</v>
@@ -2398,7 +2394,7 @@
         <v>25</v>
       </c>
       <c r="B22" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="E22" t="s">
         <v>26</v>
@@ -2409,7 +2405,7 @@
         <v>27</v>
       </c>
       <c r="B23" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="E23" t="s">
         <v>28</v>
@@ -2420,7 +2416,7 @@
         <v>29</v>
       </c>
       <c r="B24" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="E24" t="s">
         <v>30</v>
@@ -2431,7 +2427,7 @@
         <v>31</v>
       </c>
       <c r="B25" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="E25" t="s">
         <v>32</v>
@@ -2447,10 +2443,10 @@
         <v>37</v>
       </c>
       <c r="B27" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="C27" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="E27" t="s">
         <v>38</v>
@@ -2461,7 +2457,7 @@
         <v>50</v>
       </c>
       <c r="C28" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="E28" t="s">
         <v>77</v>
@@ -2493,10 +2489,10 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="C1" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="D1" t="s">
         <v>1</v>
@@ -2509,10 +2505,10 @@
     </row>
     <row r="3" spans="1:4">
       <c r="A3" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
       <c r="B3" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="D3" t="s">
         <v>54</v>
@@ -2520,10 +2516,10 @@
     </row>
     <row r="4" spans="1:4">
       <c r="A4" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
       <c r="B4" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="D4" t="s">
         <v>55</v>
@@ -2531,10 +2527,10 @@
     </row>
     <row r="5" spans="1:4">
       <c r="A5" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
       <c r="C5" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="D5" t="s">
         <v>56</v>
@@ -2542,13 +2538,13 @@
     </row>
     <row r="6" spans="1:4">
       <c r="A6" t="s">
-        <v>214</v>
+        <v>212</v>
       </c>
       <c r="B6" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="C6" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="D6" t="s">
         <v>57</v>
@@ -2556,13 +2552,13 @@
     </row>
     <row r="7" spans="1:4">
       <c r="A7" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
       <c r="B7" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="C7" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="D7" t="s">
         <v>58</v>
@@ -2575,10 +2571,10 @@
     </row>
     <row r="9" spans="1:4">
       <c r="A9" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
       <c r="B9" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="D9" t="s">
         <v>61</v>
@@ -2586,10 +2582,10 @@
     </row>
     <row r="10" spans="1:4">
       <c r="A10" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
       <c r="B10" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
       <c r="D10" t="s">
         <v>62</v>
@@ -2597,13 +2593,13 @@
     </row>
     <row r="11" spans="1:4">
       <c r="A11" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
       <c r="B11" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
       <c r="C11" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="D11" t="s">
         <v>63</v>
@@ -2611,10 +2607,10 @@
     </row>
     <row r="12" spans="1:4">
       <c r="A12" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
       <c r="B12" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="D12" t="s">
         <v>64</v>
@@ -2622,13 +2618,13 @@
     </row>
     <row r="13" spans="1:4">
       <c r="A13" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
       <c r="B13" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="C13" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="D13" t="s">
         <v>65</v>
@@ -2636,10 +2632,10 @@
     </row>
     <row r="14" spans="1:4">
       <c r="A14" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
       <c r="B14" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="D14" t="s">
         <v>66</v>
@@ -2647,10 +2643,10 @@
     </row>
     <row r="15" spans="1:4">
       <c r="A15" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
       <c r="B15" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="D15" t="s">
         <v>70</v>
@@ -2663,10 +2659,10 @@
     </row>
     <row r="17" spans="1:4">
       <c r="A17" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
       <c r="B17" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
       <c r="D17" t="s">
         <v>68</v>
@@ -2674,10 +2670,10 @@
     </row>
     <row r="18" spans="1:4">
       <c r="A18" t="s">
-        <v>194</v>
+        <v>192</v>
       </c>
       <c r="B18" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="D18" t="s">
         <v>69</v>
@@ -2685,10 +2681,10 @@
     </row>
     <row r="19" spans="1:4">
       <c r="A19" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="B19" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="D19" t="s">
         <v>72</v>
@@ -2701,10 +2697,10 @@
     </row>
     <row r="21" spans="1:4">
       <c r="A21" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
       <c r="B21" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
       <c r="D21" t="s">
         <v>75</v>
@@ -2712,13 +2708,13 @@
     </row>
     <row r="22" spans="1:4">
       <c r="A22" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
       <c r="B22" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
       <c r="C22" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="D22" t="s">
         <v>74</v>
@@ -2726,13 +2722,13 @@
     </row>
     <row r="23" spans="1:4">
       <c r="A23" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
       <c r="B23" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
       <c r="C23" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="D23" t="s">
         <v>76</v>
@@ -2740,10 +2736,10 @@
     </row>
     <row r="24" spans="1:4">
       <c r="A24" t="s">
-        <v>199</v>
+        <v>197</v>
       </c>
       <c r="B24" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
       <c r="D24" t="s">
         <v>78</v>
@@ -2751,13 +2747,13 @@
     </row>
     <row r="25" spans="1:4">
       <c r="A25" t="s">
-        <v>200</v>
+        <v>198</v>
       </c>
       <c r="B25" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
       <c r="C25" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="D25" t="s">
         <v>79</v>
@@ -2765,13 +2761,13 @@
     </row>
     <row r="26" spans="1:4">
       <c r="A26" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
       <c r="B26" s="3" t="s">
+        <v>174</v>
+      </c>
+      <c r="C26" t="s">
         <v>176</v>
-      </c>
-      <c r="C26" t="s">
-        <v>178</v>
       </c>
       <c r="D26" t="s">
         <v>80</v>

</xml_diff>